<commit_message>
Pacchetto con tutte le funzioni funzionanti. Risolto bug ebike. Aggiunti tutti i mezzi di trasporto della matrice di pendolarismo tra i mezzi di trasporto passivi
</commit_message>
<xml_diff>
--- a/data-raw/transport_speeds.xlsx
+++ b/data-raw/transport_speeds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/actmobility/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/actmobilityr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_AD4D5CB4E552A5DACE1C64C0901D4AE65BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22AEE94E-0617-40FA-8F99-EB1EA693C86A}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_AD4D5CB4E552A5DACE1C64C0901D4AE65BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A08C899E-EFA3-4A82-BBDD-F93EA7370FF5}"/>
   <bookViews>
-    <workbookView xWindow="6690" yWindow="2115" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23040" yWindow="1092" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>mean_of_transp</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>ebike</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,6 +499,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>